<commit_message>
ExcelReadList and TextReadList classes adapted to new functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Loader_i1a\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="2535"/>
   </bookViews>
@@ -10,11 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,84 +27,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>90500084Y</t>
-  </si>
-  <si>
-    <t>19160962F</t>
-  </si>
-  <si>
-    <t>09940449X</t>
-  </si>
-  <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
     <t>juan@example.com</t>
   </si>
   <si>
-    <t>luis@example.com</t>
-  </si>
-  <si>
-    <t>ana@example.com</t>
-  </si>
-  <si>
-    <t>Dirección postal</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>pollingStation</t>
+    <t>locaclizacion</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>43D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,12 +95,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -429,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,129 +396,54 @@
     <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.53138888888888891</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ExcelParseTest and TextParseTest have been adapted
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -27,37 +27,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
-    <t>juan@example.com</t>
-  </si>
-  <si>
-    <t>locaclizacion</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>kind</t>
   </si>
   <si>
-    <t>43D</t>
+    <t>locacalizacion</t>
+  </si>
+  <si>
+    <t>jorge</t>
+  </si>
+  <si>
+    <t>18:13:14:12S</t>
+  </si>
+  <si>
+    <t>jorge@email.es</t>
+  </si>
+  <si>
+    <t>ID4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,7 +110,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -386,7 +397,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,27 +415,27 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.53138888888888891</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>

<commit_message>
New improvements in tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -41,9 +41,6 @@
     <t>kind</t>
   </si>
   <si>
-    <t>locacalizacion</t>
-  </si>
-  <si>
     <t>jorge</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>ID4</t>
+  </si>
+  <si>
+    <t>localizacion</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -426,16 +426,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>